<commit_message>
we have our data sets now
</commit_message>
<xml_diff>
--- a/JaredWork/style_family.xlsx
+++ b/JaredWork/style_family.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9694b6c74c91ae88/Desktop/Bootcamp HW/CAPSTONE_PROJECT_GROUP_3/JaredWork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1A8F0A06-0252-4AEA-AE61-DF4B4CA29353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="14_{1A8F0A06-0252-4AEA-AE61-DF4B4CA29353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E32390B-BD9F-42D7-AC6D-5E1822D8091C}"/>
   <bookViews>
-    <workbookView xWindow="42450" yWindow="1290" windowWidth="23805" windowHeight="12045" xr2:uid="{8F3A3D81-83FA-4EB8-AC0C-A7C27A559BAD}"/>
+    <workbookView xWindow="-5445" yWindow="9045" windowWidth="5295" windowHeight="8655" xr2:uid="{8F3A3D81-83FA-4EB8-AC0C-A7C27A559BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Style Family</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Stout</t>
+  </si>
+  <si>
+    <t>Style_Family_ID</t>
   </si>
 </sst>
 </file>
@@ -425,79 +428,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2AA390-BB36-431A-8700-985F95A86153}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
     </row>

</xml_diff>